<commit_message>
Lagt til kontrollstrukturer med noen oppgaver. Fint mulig å bruke oppgaver fra tidligere, men passet på å legge til noen nye, kanskje litt mer utfordrende oppgaver.
Lagt til en template (ja, fra nettet, open-source) for slutt-prøven. Er bare å endre litt på språk og innhold til spørsmål.

Oppdatert timeplanen.
</commit_message>
<xml_diff>
--- a/timeplanProgKurs.xlsx
+++ b/timeplanProgKurs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strand117/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strand117/Documents/Bachelor/sommerKursProg17/SommerkursProg17/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Tid</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Fredag</t>
   </si>
   <si>
-    <t>09.00</t>
-  </si>
-  <si>
     <t>Velkommen + intro</t>
   </si>
   <si>
@@ -59,15 +56,6 @@
     <t>Programmeringsspråk</t>
   </si>
   <si>
-    <t>Variabler</t>
-  </si>
-  <si>
-    <t>Nettsider: Design</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
     <t>Fra VGS til Høgskole</t>
   </si>
   <si>
@@ -77,24 +65,12 @@
     <t>Hello World</t>
   </si>
   <si>
-    <t>11.00</t>
-  </si>
-  <si>
     <t>Kontrollstrukturer</t>
   </si>
   <si>
-    <t>Nettsider: Javascript</t>
-  </si>
-  <si>
-    <t>12.00</t>
-  </si>
-  <si>
     <t>Lunsj</t>
   </si>
   <si>
-    <t>13.00</t>
-  </si>
-  <si>
     <t>Studieteknikk</t>
   </si>
   <si>
@@ -104,23 +80,26 @@
     <t>Terminal/Konsoll</t>
   </si>
   <si>
-    <t>Nettsider: Intro</t>
-  </si>
-  <si>
-    <t>Oppsummering</t>
-  </si>
-  <si>
-    <t>14.00</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nettsider: HTML, CSS og Javascript </t>
+  </si>
+  <si>
+    <t>Intro til programmering i Java og PHP</t>
+  </si>
+  <si>
+    <t>Nettsider: Intro og design</t>
+  </si>
+  <si>
+    <t>Versjonshåndtering, oppsummering og spørsmål</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,8 +122,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,86 +147,62 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8497B0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -257,33 +227,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +530,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,190 +543,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="17">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="17">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="F4" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>13</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="17">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Pusher opp for å oppdatere master. Gjort modul 6,7,8, skal legge til litt mer innhold og fylle ut oppgaver mer nøye.
</commit_message>
<xml_diff>
--- a/timeplanProgKurs.xlsx
+++ b/timeplanProgKurs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Tid</t>
   </si>
@@ -83,16 +83,19 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Nettsider: HTML, CSS og Javascript </t>
-  </si>
-  <si>
     <t>Intro til programmering i Java og PHP</t>
   </si>
   <si>
-    <t>Nettsider: Intro og design</t>
-  </si>
-  <si>
-    <t>Versjonshåndtering, oppsummering og spørsmål</t>
+    <t>Lunsj 11:45-12:15</t>
+  </si>
+  <si>
+    <t>Nettsider intro: HTML, CSS og Javascript</t>
+  </si>
+  <si>
+    <t>Versjonshåndtering(liten intro?), oppsummering og spørsmål</t>
+  </si>
+  <si>
+    <t>Nettsider: oppbygning og brukervennlighet (+kodeoppgaver relatert til dette?)</t>
   </si>
 </sst>
 </file>
@@ -231,9 +234,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -247,6 +247,9 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -530,7 +533,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,27 +541,27 @@
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.1640625" customWidth="1"/>
     <col min="4" max="4" width="35.83203125" customWidth="1"/>
-    <col min="5" max="5" width="31.5" customWidth="1"/>
-    <col min="6" max="6" width="59" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -566,109 +569,109 @@
       <c r="A2" s="17">
         <v>9</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>18</v>
+      <c r="F4" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>11</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>12</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -676,42 +679,44 @@
       <c r="A10" s="17">
         <v>13</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
         <v>14</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -719,7 +724,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>

</xml_diff>